<commit_message>
feat: group of food
</commit_message>
<xml_diff>
--- a/references/Nutrient.xlsx
+++ b/references/Nutrient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\NutriIntel\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C233992-810A-4423-A1C3-1E265B5E14BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC01E10-5733-4331-B681-6E02E447D285}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="2910" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,7 +663,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>